<commit_message>
Version 2 de ExtractPDF
</commit_message>
<xml_diff>
--- a/CondicionesAxeso.xlsx
+++ b/CondicionesAxeso.xlsx
@@ -9,20 +9,36 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Condiciones" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -45,11 +61,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,13 +450,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.140625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="13" bestFit="1" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -456,6 +483,26 @@
           <t>cotizacion</t>
         </is>
       </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Sequence #</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>Upper Bound</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>Factor</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,7 +515,229 @@
         <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>20396</v>
+        <v>20654</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>0.1279352436098831</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="H3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>0.126940954842813</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="H4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0.1249641727581296</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="H5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>0.1234919553361154</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="H6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0.1215429015542623</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="H7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0.1210581306386495</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>0.1205743596691218</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="H9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0.1200915900996986</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="H10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I10" s="6" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0.1196098233768364</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="H11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>9000</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0.1191290609393636</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="H12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>0.1184098034467487</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="H13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>11000</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0.1176928136117802</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="H14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>12000</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>0.1375</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0.117573536107308</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="H15" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>13000</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0.1174543217474871</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="H16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0.117216082549313</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="H17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>9999999</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>0.116978096191973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>